<commit_message>
Uploaded revised category-level intensity analysis xlsx spreadsheet
</commit_message>
<xml_diff>
--- a/intensity analysis/Category_Level_Intensity_Analysis_ALL.xlsx
+++ b/intensity analysis/Category_Level_Intensity_Analysis_ALL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dondealban/Mindoro/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dondealban/Dropbox/Image Processing/Philippines/Mindoro/6 intensity analysis/2019.08.25 v4 Manuscript/2 category level/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BF1CCD-E8FD-B847-9D94-DCA83CDBA6F4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C90CF5-DB92-0E47-90A3-D168BBEE5DF9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17440" activeTab="8" xr2:uid="{542C83A6-2C42-0940-BA0F-3DA2D4557E17}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{542C83A6-2C42-0940-BA0F-3DA2D4557E17}"/>
   </bookViews>
   <sheets>
     <sheet name="Gain_Mindoro" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="Loss_MIBNP" sheetId="9" r:id="rId8"/>
     <sheet name="Gain_NLNP" sheetId="10" r:id="rId9"/>
     <sheet name="Loss_NLNP" sheetId="11" r:id="rId10"/>
+    <sheet name="Gain_SBRN" sheetId="12" r:id="rId11"/>
+    <sheet name="Loss_SBRN" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="29">
   <si>
     <t>Interval*</t>
   </si>
@@ -127,7 +129,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -182,6 +184,35 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -240,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -312,6 +343,45 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -633,9 +703,9 @@
   </sheetPr>
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -651,7 +721,7 @@
     <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,7 +756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -721,7 +791,7 @@
         <v>3.2508480548858643</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -756,7 +826,7 @@
         <v>3.2508468627929688</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -791,7 +861,7 @@
         <v>3.2508480548858643</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -826,7 +896,7 @@
         <v>3.2508468627929688</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -861,7 +931,7 @@
         <v>3.2508468627929688</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -896,7 +966,7 @@
         <v>3.2508468627929688</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -931,7 +1001,7 @@
         <v>3.2508468627929688</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -966,7 +1036,7 @@
         <v>3.2508468627929688</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1001,7 +1071,7 @@
         <v>3.9547016620635986</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -1036,7 +1106,7 @@
         <v>3.9547021389007568</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -1071,7 +1141,7 @@
         <v>3.9547016620635986</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -1106,7 +1176,7 @@
         <v>3.9547021389007568</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -1141,7 +1211,7 @@
         <v>3.9547021389007568</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -1176,7 +1246,7 @@
         <v>3.9547016620635986</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -1211,7 +1281,7 @@
         <v>3.9547021389007568</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -1246,7 +1316,7 @@
         <v>3.9547016620635986</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -1281,7 +1351,7 @@
         <v>2.4601349830627441</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -1316,7 +1386,7 @@
         <v>2.4601361751556396</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -1351,7 +1421,7 @@
         <v>2.4601349830627441</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1386,7 +1456,7 @@
         <v>2.4601349830627441</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1421,7 +1491,7 @@
         <v>2.4601361751556396</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -1456,7 +1526,7 @@
         <v>2.4601361751556396</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -1491,7 +1561,7 @@
         <v>2.4601361751556396</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>20</v>
       </c>
@@ -1538,9 +1608,11 @@
   </sheetPr>
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0"/>
+    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -1556,7 +1628,7 @@
     <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1591,7 +1663,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -1626,7 +1698,7 @@
         <v>7.1426205635070801</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1661,7 +1733,7 @@
         <v>7.1426205635070801</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1696,7 +1768,7 @@
         <v>7.1426205635070801</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1731,7 +1803,7 @@
         <v>7.1426200866699219</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1766,7 +1838,7 @@
         <v>7.1426200866699219</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -1801,7 +1873,7 @@
         <v>7.1426205635070801</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1836,7 +1908,7 @@
         <v>7.1426200866699219</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1871,7 +1943,7 @@
         <v>7.1426200866699219</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1906,7 +1978,7 @@
         <v>8.0526590347290039</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -1941,7 +2013,7 @@
         <v>8.0526590347290039</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -1976,7 +2048,7 @@
         <v>8.0526590347290039</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -2011,7 +2083,7 @@
         <v>8.0526590347290039</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -2046,7 +2118,7 @@
         <v>8.0526590347290039</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -2081,7 +2153,7 @@
         <v>8.0526590347290039</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -2116,7 +2188,7 @@
         <v>8.0526590347290039</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -2151,7 +2223,7 @@
         <v>8.0526590347290039</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -2186,7 +2258,7 @@
         <v>5.0075745582580566</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -2221,7 +2293,7 @@
         <v>5.0075745582580566</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -2256,7 +2328,7 @@
         <v>5.0075745582580566</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -2291,7 +2363,7 @@
         <v>5.0075745582580566</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -2326,7 +2398,7 @@
         <v>5.0075745582580566</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -2361,7 +2433,7 @@
         <v>5.0075745582580566</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -2396,7 +2468,7 @@
         <v>5.0075745582580566</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>20</v>
       </c>
@@ -2429,6 +2501,1605 @@
       </c>
       <c r="K25" s="18">
         <v>5.0075745582580566</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B31C39-A68B-3040-A80B-7B1AC96D5BBE}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.83203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.1640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.5" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.1640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.83203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="29">
+        <v>1</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="31">
+        <v>366.16665649414062</v>
+      </c>
+      <c r="E2" s="32">
+        <v>0.40335166454315186</v>
+      </c>
+      <c r="F2" s="33">
+        <v>0.73088151216506958</v>
+      </c>
+      <c r="G2" s="34">
+        <v>692.08660888671875</v>
+      </c>
+      <c r="H2" s="35">
+        <v>325.91995239257812</v>
+      </c>
+      <c r="I2" s="33">
+        <v>0</v>
+      </c>
+      <c r="J2" s="33">
+        <v>47.092365264892578</v>
+      </c>
+      <c r="K2" s="33">
+        <v>3.633807897567749</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="29">
+        <v>2</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="31">
+        <v>26.916666030883789</v>
+      </c>
+      <c r="E3" s="32">
+        <v>0.23409868776798248</v>
+      </c>
+      <c r="F3" s="33">
+        <v>0.73088151216506958</v>
+      </c>
+      <c r="G3" s="34">
+        <v>89.528144836425781</v>
+      </c>
+      <c r="H3" s="35">
+        <v>62.611476898193359</v>
+      </c>
+      <c r="I3" s="33">
+        <v>0</v>
+      </c>
+      <c r="J3" s="33">
+        <v>69.934967041015625</v>
+      </c>
+      <c r="K3" s="33">
+        <v>3.633807897567749</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="29">
+        <v>3</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="34">
+        <v>175.75</v>
+      </c>
+      <c r="E4" s="36">
+        <v>7.3751578330993652</v>
+      </c>
+      <c r="F4" s="33">
+        <v>0.73088151216506958</v>
+      </c>
+      <c r="G4" s="31">
+        <v>2.19512939453125</v>
+      </c>
+      <c r="H4" s="37">
+        <v>173.55487060546875</v>
+      </c>
+      <c r="I4" s="33">
+        <v>98.750991821289062</v>
+      </c>
+      <c r="J4" s="33">
+        <v>0</v>
+      </c>
+      <c r="K4" s="33">
+        <v>3.6338083744049072</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="29">
+        <v>4</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="34">
+        <v>26.333333969116211</v>
+      </c>
+      <c r="E5" s="36">
+        <v>2.29384446144104</v>
+      </c>
+      <c r="F5" s="33">
+        <v>0.73088151216506958</v>
+      </c>
+      <c r="G5" s="31">
+        <v>6.6655406951904297</v>
+      </c>
+      <c r="H5" s="37">
+        <v>19.667793273925781</v>
+      </c>
+      <c r="I5" s="33">
+        <v>74.687820434570312</v>
+      </c>
+      <c r="J5" s="33">
+        <v>0</v>
+      </c>
+      <c r="K5" s="33">
+        <v>3.6338083744049072</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="29">
+        <v>5</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="34">
+        <v>344.16665649414062</v>
+      </c>
+      <c r="E6" s="36">
+        <v>1.5211786031723022</v>
+      </c>
+      <c r="F6" s="33">
+        <v>0.73088151216506958</v>
+      </c>
+      <c r="G6" s="31">
+        <v>148.17208862304688</v>
+      </c>
+      <c r="H6" s="37">
+        <v>195.99456787109375</v>
+      </c>
+      <c r="I6" s="33">
+        <v>56.947574615478516</v>
+      </c>
+      <c r="J6" s="33">
+        <v>0</v>
+      </c>
+      <c r="K6" s="33">
+        <v>3.6338083744049072</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="29">
+        <v>6</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="38">
+        <v>0</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="33">
+        <v>0.73088151216506958</v>
+      </c>
+      <c r="G7" s="34">
+        <v>0</v>
+      </c>
+      <c r="H7" s="40">
+        <v>0</v>
+      </c>
+      <c r="I7" s="33">
+        <v>0</v>
+      </c>
+      <c r="J7" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="33">
+        <v>3.633807897567749</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="29">
+        <v>7</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="31">
+        <v>8.3333335816860199E-2</v>
+      </c>
+      <c r="E8" s="32">
+        <v>8.5910648107528687E-2</v>
+      </c>
+      <c r="F8" s="33">
+        <v>0.73088151216506958</v>
+      </c>
+      <c r="G8" s="34">
+        <v>0.7691008448600769</v>
+      </c>
+      <c r="H8" s="35">
+        <v>0.68576747179031372</v>
+      </c>
+      <c r="I8" s="33">
+        <v>0</v>
+      </c>
+      <c r="J8" s="33">
+        <v>89.164833068847656</v>
+      </c>
+      <c r="K8" s="33">
+        <v>3.633807897567749</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="29">
+        <v>1</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="31">
+        <v>450.39999389648438</v>
+      </c>
+      <c r="E9" s="32">
+        <v>0.49744319915771484</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0.9880029559135437</v>
+      </c>
+      <c r="G9" s="34">
+        <v>943.26251220703125</v>
+      </c>
+      <c r="H9" s="35">
+        <v>492.86248779296875</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0</v>
+      </c>
+      <c r="J9" s="33">
+        <v>52.250831604003906</v>
+      </c>
+      <c r="K9" s="33">
+        <v>3.8412895202636719</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="29">
+        <v>2</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="34">
+        <v>173.30000305175781</v>
+      </c>
+      <c r="E10" s="36">
+        <v>1.3491630554199219</v>
+      </c>
+      <c r="F10" s="33">
+        <v>0.9880029559135437</v>
+      </c>
+      <c r="G10" s="31">
+        <v>121.82305145263672</v>
+      </c>
+      <c r="H10" s="37">
+        <v>51.476951599121094</v>
+      </c>
+      <c r="I10" s="33">
+        <v>29.703954696655273</v>
+      </c>
+      <c r="J10" s="33">
+        <v>0</v>
+      </c>
+      <c r="K10" s="33">
+        <v>3.8412895202636719</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="29">
+        <v>3</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="34">
+        <v>51.400001525878906</v>
+      </c>
+      <c r="E11" s="36">
+        <v>4.0093603134155273</v>
+      </c>
+      <c r="F11" s="33">
+        <v>0.9880029559135437</v>
+      </c>
+      <c r="G11" s="31">
+        <v>8.4197368621826172</v>
+      </c>
+      <c r="H11" s="37">
+        <v>42.980262756347656</v>
+      </c>
+      <c r="I11" s="33">
+        <v>83.619194030761719</v>
+      </c>
+      <c r="J11" s="33">
+        <v>0</v>
+      </c>
+      <c r="K11" s="33">
+        <v>3.8412895202636719</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="29">
+        <v>4</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="34">
+        <v>131.80000305175781</v>
+      </c>
+      <c r="E12" s="36">
+        <v>6.0821409225463867</v>
+      </c>
+      <c r="F12" s="33">
+        <v>0.9880029559135437</v>
+      </c>
+      <c r="G12" s="31">
+        <v>9.3077669143676758</v>
+      </c>
+      <c r="H12" s="37">
+        <v>122.49223327636719</v>
+      </c>
+      <c r="I12" s="33">
+        <v>92.937965393066406</v>
+      </c>
+      <c r="J12" s="33">
+        <v>0</v>
+      </c>
+      <c r="K12" s="33">
+        <v>3.8412895202636719</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="29">
+        <v>5</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="34">
+        <v>463</v>
+      </c>
+      <c r="E13" s="36">
+        <v>2.1419320106506348</v>
+      </c>
+      <c r="F13" s="33">
+        <v>0.9880029559135437</v>
+      </c>
+      <c r="G13" s="31">
+        <v>186.2208251953125</v>
+      </c>
+      <c r="H13" s="37">
+        <v>276.7791748046875</v>
+      </c>
+      <c r="I13" s="33">
+        <v>59.779518127441406</v>
+      </c>
+      <c r="J13" s="33">
+        <v>0</v>
+      </c>
+      <c r="K13" s="33">
+        <v>3.8412895202636719</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="29">
+        <v>6</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="38">
+        <v>0</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="33">
+        <v>0.9880029559135437</v>
+      </c>
+      <c r="G14" s="34">
+        <v>0</v>
+      </c>
+      <c r="H14" s="40">
+        <v>0</v>
+      </c>
+      <c r="I14" s="33">
+        <v>0</v>
+      </c>
+      <c r="J14" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="33">
+        <v>3.8412895202636719</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="29">
+        <v>7</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="31">
+        <v>0</v>
+      </c>
+      <c r="E15" s="32">
+        <v>0</v>
+      </c>
+      <c r="F15" s="33">
+        <v>0.9880029559135437</v>
+      </c>
+      <c r="G15" s="34">
+        <v>0.8660925030708313</v>
+      </c>
+      <c r="H15" s="35">
+        <v>0.8660925030708313</v>
+      </c>
+      <c r="I15" s="33">
+        <v>0</v>
+      </c>
+      <c r="J15" s="33">
+        <v>100</v>
+      </c>
+      <c r="K15" s="33">
+        <v>3.8412895202636719</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="29">
+        <v>1</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="31">
+        <v>860.79998779296875</v>
+      </c>
+      <c r="E16" s="32">
+        <v>0.9694676399230957</v>
+      </c>
+      <c r="F16" s="33">
+        <v>2.0978434085845947</v>
+      </c>
+      <c r="G16" s="34">
+        <v>1980.1021728515625</v>
+      </c>
+      <c r="H16" s="35">
+        <v>1119.3021240234375</v>
+      </c>
+      <c r="I16" s="33">
+        <v>0</v>
+      </c>
+      <c r="J16" s="33">
+        <v>56.527496337890625</v>
+      </c>
+      <c r="K16" s="33">
+        <v>4.456385612487793</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="29">
+        <v>2</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="31">
+        <v>249.60000610351562</v>
+      </c>
+      <c r="E17" s="32">
+        <v>1.9171979427337646</v>
+      </c>
+      <c r="F17" s="33">
+        <v>2.0978434085845947</v>
+      </c>
+      <c r="G17" s="34">
+        <v>275.87420654296875</v>
+      </c>
+      <c r="H17" s="35">
+        <v>26.274190902709961</v>
+      </c>
+      <c r="I17" s="33">
+        <v>0</v>
+      </c>
+      <c r="J17" s="33">
+        <v>9.5239753723144531</v>
+      </c>
+      <c r="K17" s="33">
+        <v>4.456385612487793</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="29">
+        <v>3</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="34">
+        <v>187.19999694824219</v>
+      </c>
+      <c r="E18" s="36">
+        <v>12.405566215515137</v>
+      </c>
+      <c r="F18" s="33">
+        <v>2.0978434085845947</v>
+      </c>
+      <c r="G18" s="31">
+        <v>13.429269790649414</v>
+      </c>
+      <c r="H18" s="37">
+        <v>173.77072143554688</v>
+      </c>
+      <c r="I18" s="33">
+        <v>92.826240539550781</v>
+      </c>
+      <c r="J18" s="33">
+        <v>0</v>
+      </c>
+      <c r="K18" s="33">
+        <v>4.4563851356506348</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="29">
+        <v>4</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="34">
+        <v>25.200000762939453</v>
+      </c>
+      <c r="E19" s="36">
+        <v>2.6780021190643311</v>
+      </c>
+      <c r="F19" s="33">
+        <v>2.0978434085845947</v>
+      </c>
+      <c r="G19" s="31">
+        <v>19.10096549987793</v>
+      </c>
+      <c r="H19" s="37">
+        <v>6.099034309387207</v>
+      </c>
+      <c r="I19" s="33">
+        <v>24.202518463134766</v>
+      </c>
+      <c r="J19" s="33">
+        <v>0</v>
+      </c>
+      <c r="K19" s="33">
+        <v>4.4563851356506348</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="29">
+        <v>5</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="34">
+        <v>1366.199951171875</v>
+      </c>
+      <c r="E20" s="36">
+        <v>5.6515264511108398</v>
+      </c>
+      <c r="F20" s="33">
+        <v>2.0978434085845947</v>
+      </c>
+      <c r="G20" s="31">
+        <v>406.46380615234375</v>
+      </c>
+      <c r="H20" s="37">
+        <v>959.73614501953125</v>
+      </c>
+      <c r="I20" s="33">
+        <v>70.248580932617188</v>
+      </c>
+      <c r="J20" s="33">
+        <v>0</v>
+      </c>
+      <c r="K20" s="33">
+        <v>4.4563851356506348</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="29">
+        <v>6</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="34">
+        <v>5.5999999046325684</v>
+      </c>
+      <c r="E21" s="36">
+        <v>20</v>
+      </c>
+      <c r="F21" s="33">
+        <v>2.0978434085845947</v>
+      </c>
+      <c r="G21" s="31">
+        <v>-9.5367433061710472E-8</v>
+      </c>
+      <c r="H21" s="37">
+        <v>5.5999999046325684</v>
+      </c>
+      <c r="I21" s="33">
+        <v>100</v>
+      </c>
+      <c r="J21" s="33">
+        <v>0</v>
+      </c>
+      <c r="K21" s="33">
+        <v>4.4563851356506348</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="29">
+        <v>7</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="34">
+        <v>1.7999999523162842</v>
+      </c>
+      <c r="E22" s="36">
+        <v>2.5714285373687744</v>
+      </c>
+      <c r="F22" s="33">
+        <v>2.0978434085845947</v>
+      </c>
+      <c r="G22" s="31">
+        <v>1.4296427965164185</v>
+      </c>
+      <c r="H22" s="37">
+        <v>0.37035715579986572</v>
+      </c>
+      <c r="I22" s="33">
+        <v>20.575397491455078</v>
+      </c>
+      <c r="J22" s="33">
+        <v>0</v>
+      </c>
+      <c r="K22" s="33">
+        <v>4.4563851356506348</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C697E359-9165-9442-9506-373F5D0E4FF8}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="29">
+        <v>1</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="16">
+        <v>286.66665649414062</v>
+      </c>
+      <c r="E2" s="17">
+        <v>0.31913197040557861</v>
+      </c>
+      <c r="F2" s="18">
+        <v>0.73088151216506958</v>
+      </c>
+      <c r="G2" s="19">
+        <v>692.08660888671875</v>
+      </c>
+      <c r="H2" s="20">
+        <v>405.419921875</v>
+      </c>
+      <c r="I2" s="18">
+        <v>0</v>
+      </c>
+      <c r="J2" s="18">
+        <v>58.579364776611328</v>
+      </c>
+      <c r="K2" s="18">
+        <v>3.7850799560546875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="29">
+        <v>2</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="19">
+        <v>259.41665649414062</v>
+      </c>
+      <c r="E3" s="21">
+        <v>1.8156261444091797</v>
+      </c>
+      <c r="F3" s="18">
+        <v>0.73088151216506958</v>
+      </c>
+      <c r="G3" s="16">
+        <v>89.52813720703125</v>
+      </c>
+      <c r="H3" s="23">
+        <v>169.88851928710938</v>
+      </c>
+      <c r="I3" s="18">
+        <v>65.488670349121094</v>
+      </c>
+      <c r="J3" s="18">
+        <v>0</v>
+      </c>
+      <c r="K3" s="18">
+        <v>3.7850806713104248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="29">
+        <v>3</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="19">
+        <v>8.1666669845581055</v>
+      </c>
+      <c r="E4" s="21">
+        <v>2.1953403949737549</v>
+      </c>
+      <c r="F4" s="18">
+        <v>0.73088151216506958</v>
+      </c>
+      <c r="G4" s="16">
+        <v>2.1951425075531006</v>
+      </c>
+      <c r="H4" s="23">
+        <v>5.971524715423584</v>
+      </c>
+      <c r="I4" s="18">
+        <v>73.120712280273438</v>
+      </c>
+      <c r="J4" s="18">
+        <v>0</v>
+      </c>
+      <c r="K4" s="18">
+        <v>3.7850806713104248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="29">
+        <v>4</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="19">
+        <v>89.5</v>
+      </c>
+      <c r="E5" s="21">
+        <v>4.6956977844238281</v>
+      </c>
+      <c r="F5" s="18">
+        <v>0.73088151216506958</v>
+      </c>
+      <c r="G5" s="16">
+        <v>6.6655426025390625</v>
+      </c>
+      <c r="H5" s="23">
+        <v>82.834457397460938</v>
+      </c>
+      <c r="I5" s="18">
+        <v>92.552467346191406</v>
+      </c>
+      <c r="J5" s="18">
+        <v>0</v>
+      </c>
+      <c r="K5" s="18">
+        <v>3.7850806713104248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="29">
+        <v>5</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="19">
+        <v>273.25</v>
+      </c>
+      <c r="E6" s="21">
+        <v>1.2549370527267456</v>
+      </c>
+      <c r="F6" s="18">
+        <v>0.73088151216506958</v>
+      </c>
+      <c r="G6" s="16">
+        <v>148.17208862304688</v>
+      </c>
+      <c r="H6" s="23">
+        <v>125.07791137695312</v>
+      </c>
+      <c r="I6" s="18">
+        <v>45.774166107177734</v>
+      </c>
+      <c r="J6" s="18">
+        <v>0</v>
+      </c>
+      <c r="K6" s="18">
+        <v>3.7850806713104248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="29">
+        <v>6</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="19">
+        <v>11.333333015441895</v>
+      </c>
+      <c r="E7" s="21">
+        <v>8.3333330154418945</v>
+      </c>
+      <c r="F7" s="18">
+        <v>0.73088151216506958</v>
+      </c>
+      <c r="G7" s="16">
+        <v>-3.1789144827598648E-7</v>
+      </c>
+      <c r="H7" s="23">
+        <v>11.333333015441895</v>
+      </c>
+      <c r="I7" s="18">
+        <v>100</v>
+      </c>
+      <c r="J7" s="18">
+        <v>0</v>
+      </c>
+      <c r="K7" s="18">
+        <v>3.7850806713104248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="29">
+        <v>7</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="19">
+        <v>11.083333015441895</v>
+      </c>
+      <c r="E8" s="21">
+        <v>4.8398833274841309</v>
+      </c>
+      <c r="F8" s="18">
+        <v>0.73088151216506958</v>
+      </c>
+      <c r="G8" s="16">
+        <v>0.76910114288330078</v>
+      </c>
+      <c r="H8" s="23">
+        <v>10.314231872558594</v>
+      </c>
+      <c r="I8" s="18">
+        <v>93.060737609863281</v>
+      </c>
+      <c r="J8" s="18">
+        <v>0</v>
+      </c>
+      <c r="K8" s="18">
+        <v>3.7850806713104248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="29">
+        <v>1</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="16">
+        <v>474.20001220703125</v>
+      </c>
+      <c r="E9" s="17">
+        <v>0.52235597372055054</v>
+      </c>
+      <c r="F9" s="18">
+        <v>0.9880029559135437</v>
+      </c>
+      <c r="G9" s="19">
+        <v>943.26251220703125</v>
+      </c>
+      <c r="H9" s="20">
+        <v>469.0625</v>
+      </c>
+      <c r="I9" s="18">
+        <v>0</v>
+      </c>
+      <c r="J9" s="18">
+        <v>49.727672576904297</v>
+      </c>
+      <c r="K9" s="18">
+        <v>4.2968721389770508</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="29">
+        <v>2</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="16">
+        <v>38.599998474121094</v>
+      </c>
+      <c r="E10" s="17">
+        <v>0.3357105553150177</v>
+      </c>
+      <c r="F10" s="18">
+        <v>0.9880029559135437</v>
+      </c>
+      <c r="G10" s="19">
+        <v>121.82304382324219</v>
+      </c>
+      <c r="H10" s="20">
+        <v>83.223037719726562</v>
+      </c>
+      <c r="I10" s="18">
+        <v>0</v>
+      </c>
+      <c r="J10" s="18">
+        <v>68.314697265625</v>
+      </c>
+      <c r="K10" s="18">
+        <v>4.2968721389770508</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="29">
+        <v>3</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="19">
+        <v>161.5</v>
+      </c>
+      <c r="E11" s="21">
+        <v>6.7771711349487305</v>
+      </c>
+      <c r="F11" s="18">
+        <v>0.9880029559135437</v>
+      </c>
+      <c r="G11" s="16">
+        <v>8.4197511672973633</v>
+      </c>
+      <c r="H11" s="23">
+        <v>153.08024597167969</v>
+      </c>
+      <c r="I11" s="18">
+        <v>94.786529541015625</v>
+      </c>
+      <c r="J11" s="18">
+        <v>0</v>
+      </c>
+      <c r="K11" s="18">
+        <v>4.2968721389770508</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="29">
+        <v>4</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="19">
+        <v>29.899999618530273</v>
+      </c>
+      <c r="E12" s="21">
+        <v>2.6045296192169189</v>
+      </c>
+      <c r="F12" s="18">
+        <v>0.9880029559135437</v>
+      </c>
+      <c r="G12" s="16">
+        <v>9.3077545166015625</v>
+      </c>
+      <c r="H12" s="23">
+        <v>20.592245101928711</v>
+      </c>
+      <c r="I12" s="18">
+        <v>68.870384216308594</v>
+      </c>
+      <c r="J12" s="18">
+        <v>0</v>
+      </c>
+      <c r="K12" s="18">
+        <v>4.2968721389770508</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="29">
+        <v>5</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="19">
+        <v>563.9000244140625</v>
+      </c>
+      <c r="E13" s="21">
+        <v>2.4923758506774902</v>
+      </c>
+      <c r="F13" s="18">
+        <v>0.9880029559135437</v>
+      </c>
+      <c r="G13" s="16">
+        <v>186.22085571289062</v>
+      </c>
+      <c r="H13" s="23">
+        <v>377.67916870117188</v>
+      </c>
+      <c r="I13" s="18">
+        <v>66.976264953613281</v>
+      </c>
+      <c r="J13" s="18">
+        <v>0</v>
+      </c>
+      <c r="K13" s="18">
+        <v>4.2968721389770508</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="29">
+        <v>6</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="24">
+        <v>0</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="18">
+        <v>0.9880029559135437</v>
+      </c>
+      <c r="G14" s="19">
+        <v>0</v>
+      </c>
+      <c r="H14" s="26">
+        <v>0</v>
+      </c>
+      <c r="I14" s="18">
+        <v>0</v>
+      </c>
+      <c r="J14" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="18">
+        <v>4.2968721389770508</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="29">
+        <v>7</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="19">
+        <v>1.7999999523162842</v>
+      </c>
+      <c r="E15" s="21">
+        <v>1.8556702136993408</v>
+      </c>
+      <c r="F15" s="18">
+        <v>0.9880029559135437</v>
+      </c>
+      <c r="G15" s="16">
+        <v>0.86609232425689697</v>
+      </c>
+      <c r="H15" s="23">
+        <v>0.93390762805938721</v>
+      </c>
+      <c r="I15" s="18">
+        <v>51.883754730224609</v>
+      </c>
+      <c r="J15" s="18">
+        <v>0</v>
+      </c>
+      <c r="K15" s="18">
+        <v>4.2968721389770508</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="29">
+        <v>1</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="16">
+        <v>1211.199951171875</v>
+      </c>
+      <c r="E16" s="17">
+        <v>1.3377069234848022</v>
+      </c>
+      <c r="F16" s="18">
+        <v>2.0978434085845947</v>
+      </c>
+      <c r="G16" s="19">
+        <v>1980.1021728515625</v>
+      </c>
+      <c r="H16" s="20">
+        <v>768.9022216796875</v>
+      </c>
+      <c r="I16" s="18">
+        <v>0</v>
+      </c>
+      <c r="J16" s="18">
+        <v>38.831439971923828</v>
+      </c>
+      <c r="K16" s="18">
+        <v>3.2286760807037354</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="29">
+        <v>2</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="16">
+        <v>214.80000305175781</v>
+      </c>
+      <c r="E17" s="17">
+        <v>1.672245979309082</v>
+      </c>
+      <c r="F17" s="18">
+        <v>2.0978434085845947</v>
+      </c>
+      <c r="G17" s="19">
+        <v>275.87420654296875</v>
+      </c>
+      <c r="H17" s="20">
+        <v>61.074195861816406</v>
+      </c>
+      <c r="I17" s="18">
+        <v>0</v>
+      </c>
+      <c r="J17" s="18">
+        <v>22.138422012329102</v>
+      </c>
+      <c r="K17" s="18">
+        <v>3.2286760807037354</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="29">
+        <v>3</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="19">
+        <v>141.80000305175781</v>
+      </c>
+      <c r="E18" s="21">
+        <v>11.060842514038086</v>
+      </c>
+      <c r="F18" s="18">
+        <v>2.0978434085845947</v>
+      </c>
+      <c r="G18" s="16">
+        <v>13.429275512695312</v>
+      </c>
+      <c r="H18" s="23">
+        <v>128.3707275390625</v>
+      </c>
+      <c r="I18" s="18">
+        <v>90.529426574707031</v>
+      </c>
+      <c r="J18" s="18">
+        <v>0</v>
+      </c>
+      <c r="K18" s="18">
+        <v>3.2286751270294189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="29">
+        <v>4</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="19">
+        <v>270.39999389648438</v>
+      </c>
+      <c r="E19" s="21">
+        <v>12.478079795837402</v>
+      </c>
+      <c r="F19" s="18">
+        <v>2.0978434085845947</v>
+      </c>
+      <c r="G19" s="16">
+        <v>19.100971221923828</v>
+      </c>
+      <c r="H19" s="23">
+        <v>251.29902648925781</v>
+      </c>
+      <c r="I19" s="18">
+        <v>92.936027526855469</v>
+      </c>
+      <c r="J19" s="18">
+        <v>0</v>
+      </c>
+      <c r="K19" s="18">
+        <v>3.2286751270294189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="29">
+        <v>5</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="19">
+        <v>854.5999755859375</v>
+      </c>
+      <c r="E20" s="21">
+        <v>3.9535529613494873</v>
+      </c>
+      <c r="F20" s="18">
+        <v>2.0978434085845947</v>
+      </c>
+      <c r="G20" s="16">
+        <v>406.46383666992188</v>
+      </c>
+      <c r="H20" s="23">
+        <v>448.13613891601562</v>
+      </c>
+      <c r="I20" s="18">
+        <v>52.438114166259766</v>
+      </c>
+      <c r="J20" s="18">
+        <v>0</v>
+      </c>
+      <c r="K20" s="18">
+        <v>3.2286751270294189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="29">
+        <v>6</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="24">
+        <v>0</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="18">
+        <v>2.0978434085845947</v>
+      </c>
+      <c r="G21" s="19">
+        <v>0</v>
+      </c>
+      <c r="H21" s="26">
+        <v>0</v>
+      </c>
+      <c r="I21" s="18">
+        <v>0</v>
+      </c>
+      <c r="J21" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="18">
+        <v>3.2286760807037354</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="29">
+        <v>7</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="19">
+        <v>3.5999999046325684</v>
+      </c>
+      <c r="E22" s="21">
+        <v>4.5569620132446289</v>
+      </c>
+      <c r="F22" s="18">
+        <v>2.0978434085845947</v>
+      </c>
+      <c r="G22" s="16">
+        <v>1.4296427965164185</v>
+      </c>
+      <c r="H22" s="23">
+        <v>2.1703572273254395</v>
+      </c>
+      <c r="I22" s="18">
+        <v>60.287696838378906</v>
+      </c>
+      <c r="J22" s="18">
+        <v>0</v>
+      </c>
+      <c r="K22" s="18">
+        <v>3.2286751270294189</v>
       </c>
     </row>
   </sheetData>
@@ -2445,7 +4116,7 @@
   <sheetViews>
     <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -2461,7 +4132,7 @@
     <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2496,7 +4167,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -2531,7 +4202,7 @@
         <v>3.9298391342163086</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -2566,7 +4237,7 @@
         <v>3.9298379421234131</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -2601,7 +4272,7 @@
         <v>3.9298379421234131</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -2636,7 +4307,7 @@
         <v>3.9298379421234131</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -2671,7 +4342,7 @@
         <v>3.9298379421234131</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -2706,7 +4377,7 @@
         <v>3.9298391342163086</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -2741,7 +4412,7 @@
         <v>3.9298379421234131</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -2776,7 +4447,7 @@
         <v>3.9298391342163086</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -2811,7 +4482,7 @@
         <v>3.2864193916320801</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -2846,7 +4517,7 @@
         <v>3.2864201068878174</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -2881,7 +4552,7 @@
         <v>3.2864193916320801</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -2916,7 +4587,7 @@
         <v>3.2864193916320801</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -2951,7 +4622,7 @@
         <v>3.2864201068878174</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -2986,7 +4657,7 @@
         <v>3.2864201068878174</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -3021,7 +4692,7 @@
         <v>3.2864201068878174</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -3056,7 +4727,7 @@
         <v>3.2864193916320801</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -3091,7 +4762,7 @@
         <v>2.9402737617492676</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -3126,7 +4797,7 @@
         <v>2.9402737617492676</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -3161,7 +4832,7 @@
         <v>2.9402735233306885</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -3196,7 +4867,7 @@
         <v>2.9402737617492676</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -3231,7 +4902,7 @@
         <v>2.9402737617492676</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -3266,7 +4937,7 @@
         <v>2.9402735233306885</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -3301,7 +4972,7 @@
         <v>2.9402737617492676</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>20</v>
       </c>
@@ -3350,7 +5021,7 @@
   <sheetViews>
     <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -3366,7 +5037,7 @@
     <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3401,7 +5072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -3436,7 +5107,7 @@
         <v>4.5578058809041977E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -3471,7 +5142,7 @@
         <v>4.5578058809041977E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -3506,7 +5177,7 @@
         <v>4.5578058809041977E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -3541,7 +5212,7 @@
         <v>4.5578058809041977E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -3576,7 +5247,7 @@
         <v>4.5578058809041977E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -3611,7 +5282,7 @@
         <v>4.5578058809041977E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -3646,7 +5317,7 @@
         <v>4.5578058809041977E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -3681,7 +5352,7 @@
         <v>4.5578058809041977E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -3716,7 +5387,7 @@
         <v>2.1830810233950615E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -3751,7 +5422,7 @@
         <v>2.1830810233950615E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -3786,7 +5457,7 @@
         <v>2.1830810233950615E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -3821,7 +5492,7 @@
         <v>2.1830810233950615E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -3856,7 +5527,7 @@
         <v>2.1830810233950615E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -3891,7 +5562,7 @@
         <v>2.1830810233950615E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -3926,7 +5597,7 @@
         <v>2.1830810233950615E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -3961,7 +5632,7 @@
         <v>2.1830810233950615E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -3996,7 +5667,7 @@
         <v>8.2240896299481392E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -4031,7 +5702,7 @@
         <v>8.2240896299481392E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -4066,7 +5737,7 @@
         <v>8.2240896299481392E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -4101,7 +5772,7 @@
         <v>8.2240896299481392E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -4136,7 +5807,7 @@
         <v>8.2240896299481392E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -4171,7 +5842,7 @@
         <v>8.2240896299481392E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -4206,7 +5877,7 @@
         <v>8.2240896299481392E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>20</v>
       </c>
@@ -4255,7 +5926,7 @@
   <sheetViews>
     <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -4271,7 +5942,7 @@
     <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4306,7 +5977,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -4341,7 +6012,7 @@
         <v>4.5261535793542862E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -4376,7 +6047,7 @@
         <v>4.5261528342962265E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -4411,7 +6082,7 @@
         <v>4.5261535793542862E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -4446,7 +6117,7 @@
         <v>4.5261528342962265E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -4481,7 +6152,7 @@
         <v>4.5261535793542862E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -4516,7 +6187,7 @@
         <v>4.5261535793542862E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -4551,7 +6222,7 @@
         <v>4.5261528342962265E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -4586,7 +6257,7 @@
         <v>4.5261535793542862E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -4621,7 +6292,7 @@
         <v>2.753121592104435E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -4656,7 +6327,7 @@
         <v>2.753121592104435E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -4691,7 +6362,7 @@
         <v>2.753121592104435E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -4726,7 +6397,7 @@
         <v>2.753121592104435E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -4761,7 +6432,7 @@
         <v>2.753121592104435E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -4796,7 +6467,7 @@
         <v>2.753121592104435E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -4831,7 +6502,7 @@
         <v>2.753121592104435E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -4866,7 +6537,7 @@
         <v>2.753121592104435E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -4901,7 +6572,7 @@
         <v>1.0440833866596222E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -4936,7 +6607,7 @@
         <v>1.0440832935273647E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -4971,7 +6642,7 @@
         <v>1.0440833866596222E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -5006,7 +6677,7 @@
         <v>1.0440832935273647E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -5041,7 +6712,7 @@
         <v>1.0440833866596222E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -5076,7 +6747,7 @@
         <v>1.0440833866596222E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -5111,7 +6782,7 @@
         <v>1.0440832935273647E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>20</v>
       </c>
@@ -5160,7 +6831,7 @@
   <sheetViews>
     <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -5176,7 +6847,7 @@
     <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5211,7 +6882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -5246,7 +6917,7 @@
         <v>5.3685593605041504</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -5281,7 +6952,7 @@
         <v>5.3685593605041504</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -5316,7 +6987,7 @@
         <v>5.3685574531555176</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -5351,7 +7022,7 @@
         <v>5.3685574531555176</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -5386,7 +7057,7 @@
         <v>5.3685574531555176</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -5421,7 +7092,7 @@
         <v>5.3685574531555176</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -5456,7 +7127,7 @@
         <v>5.3685574531555176</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -5491,7 +7162,7 @@
         <v>5.3685593605041504</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -5526,7 +7197,7 @@
         <v>1.7578459978103638</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -5561,7 +7232,7 @@
         <v>1.7578459978103638</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -5596,7 +7267,7 @@
         <v>1.757846474647522</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -5631,7 +7302,7 @@
         <v>1.7578459978103638</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -5666,7 +7337,7 @@
         <v>1.7578459978103638</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -5701,7 +7372,7 @@
         <v>1.757846474647522</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -5736,7 +7407,7 @@
         <v>1.7578459978103638</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -5771,7 +7442,7 @@
         <v>1.757846474647522</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -5806,7 +7477,7 @@
         <v>5.1848306655883789</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -5841,7 +7512,7 @@
         <v>5.1848306655883789</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -5876,7 +7547,7 @@
         <v>5.1848306655883789</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -5911,7 +7582,7 @@
         <v>5.1848297119140625</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -5946,7 +7617,7 @@
         <v>5.1848297119140625</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -5981,7 +7652,7 @@
         <v>5.1848297119140625</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -6016,7 +7687,7 @@
         <v>5.1848297119140625</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>20</v>
       </c>
@@ -6065,7 +7736,7 @@
   <sheetViews>
     <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -6081,7 +7752,7 @@
     <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6116,7 +7787,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -6151,7 +7822,7 @@
         <v>4.4105801582336426</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -6186,7 +7857,7 @@
         <v>4.4105796813964844</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -6221,7 +7892,7 @@
         <v>4.4105801582336426</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -6256,7 +7927,7 @@
         <v>4.4105796813964844</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -6291,7 +7962,7 @@
         <v>4.4105796813964844</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -6326,7 +7997,7 @@
         <v>4.4105801582336426</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -6361,7 +8032,7 @@
         <v>4.4105796813964844</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -6396,7 +8067,7 @@
         <v>4.4105801582336426</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -6431,7 +8102,7 @@
         <v>2.5125346183776855</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -6466,7 +8137,7 @@
         <v>2.51253342628479</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -6501,7 +8172,7 @@
         <v>2.51253342628479</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -6536,7 +8207,7 @@
         <v>2.51253342628479</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -6571,7 +8242,7 @@
         <v>2.51253342628479</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -6606,7 +8277,7 @@
         <v>2.5125346183776855</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -6641,7 +8312,7 @@
         <v>2.51253342628479</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -6676,7 +8347,7 @@
         <v>2.5125346183776855</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -6711,7 +8382,7 @@
         <v>5.7456488609313965</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -6746,7 +8417,7 @@
         <v>5.7456488609313965</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -6781,7 +8452,7 @@
         <v>5.7456488609313965</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -6816,7 +8487,7 @@
         <v>5.7456488609313965</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -6851,7 +8522,7 @@
         <v>5.7456488609313965</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -6886,7 +8557,7 @@
         <v>5.7456479072570801</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -6921,7 +8592,7 @@
         <v>5.7456488609313965</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>20</v>
       </c>
@@ -6970,7 +8641,7 @@
   <sheetViews>
     <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -6986,7 +8657,7 @@
     <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7021,7 +8692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -7056,7 +8727,7 @@
         <v>4.9035911560058594</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -7091,7 +8762,7 @@
         <v>4.9035921096801758</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -7126,7 +8797,7 @@
         <v>4.9035911560058594</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -7161,7 +8832,7 @@
         <v>4.9035921096801758</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -7196,7 +8867,7 @@
         <v>4.9035921096801758</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -7231,7 +8902,7 @@
         <v>4.9035921096801758</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -7266,7 +8937,7 @@
         <v>4.9035911560058594</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -7301,7 +8972,7 @@
         <v>4.9035921096801758</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -7336,7 +9007,7 @@
         <v>2.2096438407897949</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -7371,7 +9042,7 @@
         <v>2.2096438407897949</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -7406,7 +9077,7 @@
         <v>2.2096438407897949</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -7441,7 +9112,7 @@
         <v>2.2096436023712158</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -7476,7 +9147,7 @@
         <v>2.2096436023712158</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -7511,7 +9182,7 @@
         <v>2.2096436023712158</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -7546,7 +9217,7 @@
         <v>2.2096436023712158</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -7581,7 +9252,7 @@
         <v>2.2096438407897949</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -7616,7 +9287,7 @@
         <v>5.329869270324707</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -7651,7 +9322,7 @@
         <v>5.329869270324707</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -7686,7 +9357,7 @@
         <v>5.329869270324707</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -7721,7 +9392,7 @@
         <v>5.3298707008361816</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -7756,7 +9427,7 @@
         <v>5.3298707008361816</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -7791,7 +9462,7 @@
         <v>5.3298707008361816</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -7826,7 +9497,7 @@
         <v>5.3298707008361816</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>20</v>
       </c>
@@ -7875,7 +9546,7 @@
   <sheetViews>
     <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -7891,7 +9562,7 @@
     <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7926,7 +9597,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -7961,7 +9632,7 @@
         <v>1.7494622468948364</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -7996,7 +9667,7 @@
         <v>1.7494627237319946</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -8031,7 +9702,7 @@
         <v>1.7494627237319946</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -8066,7 +9737,7 @@
         <v>1.7494627237319946</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -8101,7 +9772,7 @@
         <v>1.7494627237319946</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -8136,7 +9807,7 @@
         <v>1.7494627237319946</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -8171,7 +9842,7 @@
         <v>1.7494627237319946</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -8206,7 +9877,7 @@
         <v>1.7494622468948364</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -8241,7 +9912,7 @@
         <v>3.6313743591308594</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -8276,7 +9947,7 @@
         <v>3.6313748359680176</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -8311,7 +9982,7 @@
         <v>3.6313743591308594</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -8346,7 +10017,7 @@
         <v>3.6313748359680176</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -8381,7 +10052,7 @@
         <v>3.6313748359680176</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -8416,7 +10087,7 @@
         <v>3.6313748359680176</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -8451,7 +10122,7 @@
         <v>3.6313743591308594</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -8486,7 +10157,7 @@
         <v>3.6313748359680176</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -8521,7 +10192,7 @@
         <v>2.5184433460235596</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -8556,7 +10227,7 @@
         <v>2.5184423923492432</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -8591,7 +10262,7 @@
         <v>2.5184423923492432</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -8626,7 +10297,7 @@
         <v>2.5184433460235596</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -8661,7 +10332,7 @@
         <v>2.5184433460235596</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -8696,7 +10367,7 @@
         <v>2.5184433460235596</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -8731,7 +10402,7 @@
         <v>2.5184433460235596</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>20</v>
       </c>
@@ -8778,9 +10449,9 @@
   </sheetPr>
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0"/>
+    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -8796,7 +10467,7 @@
     <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8831,7 +10502,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -8866,7 +10537,7 @@
         <v>6.0556831359863281</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -8901,7 +10572,7 @@
         <v>6.0556831359863281</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -8936,7 +10607,7 @@
         <v>6.0556831359863281</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -8971,7 +10642,7 @@
         <v>6.0556831359863281</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -9006,7 +10677,7 @@
         <v>6.0556831359863281</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -9041,7 +10712,7 @@
         <v>6.0556831359863281</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -9076,7 +10747,7 @@
         <v>6.0556831359863281</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -9111,7 +10782,7 @@
         <v>6.0556831359863281</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -9146,7 +10817,7 @@
         <v>6.3604164123535156</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -9181,7 +10852,7 @@
         <v>6.3604164123535156</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -9216,7 +10887,7 @@
         <v>6.3604164123535156</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -9251,7 +10922,7 @@
         <v>6.3604164123535156</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -9286,7 +10957,7 @@
         <v>6.3604164123535156</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -9321,7 +10992,7 @@
         <v>6.3604164123535156</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -9356,7 +11027,7 @@
         <v>6.3604164123535156</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -9391,7 +11062,7 @@
         <v>6.3604164123535156</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -9426,7 +11097,7 @@
         <v>3.7319095134735107</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -9461,7 +11132,7 @@
         <v>3.7319095134735107</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -9496,7 +11167,7 @@
         <v>3.7319095134735107</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -9531,7 +11202,7 @@
         <v>3.7319095134735107</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -9566,7 +11237,7 @@
         <v>3.7319095134735107</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -9601,7 +11272,7 @@
         <v>3.7319095134735107</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -9636,7 +11307,7 @@
         <v>3.7319095134735107</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>20</v>
       </c>

</xml_diff>